<commit_message>
Added more provinces to file
</commit_message>
<xml_diff>
--- a/MapFiles/ProvinceInfoExcel.xlsx
+++ b/MapFiles/ProvinceInfoExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redss\Desktop\APPDEV\Tauresium\MapFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB36D6B-AB79-4A9E-A9E8-5BBDF0FA7DAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C631B2DC-1A55-485A-B79E-7F745F473ADA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1BFF37CF-5075-4621-9872-3602807B8ECF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1BFF37CF-5075-4621-9872-3602807B8ECF}"/>
   </bookViews>
   <sheets>
     <sheet name="Provinces" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="1096">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2243" uniqueCount="1151">
   <si>
     <t>Alaska_BristolBay</t>
   </si>
@@ -3323,6 +3323,171 @@
   </si>
   <si>
     <t>Atar</t>
+  </si>
+  <si>
+    <t>America West</t>
+  </si>
+  <si>
+    <t>Laayoune</t>
+  </si>
+  <si>
+    <t>West Sahara</t>
+  </si>
+  <si>
+    <t>Khartoum</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Port Sudan</t>
+  </si>
+  <si>
+    <t>Al-Ubayyid</t>
+  </si>
+  <si>
+    <t>Asmara</t>
+  </si>
+  <si>
+    <t>Yaounde</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Kuala Lumpur</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Phnom Penh</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Vientiane</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Nur-Sultan</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Aktau</t>
+  </si>
+  <si>
+    <t>Addis Ababa</t>
+  </si>
+  <si>
+    <t>Oromiya</t>
+  </si>
+  <si>
+    <t>Somali</t>
+  </si>
+  <si>
+    <t>Jigjiga</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Horn Of Africa</t>
+  </si>
+  <si>
+    <t>Nairobi</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Mombasa</t>
+  </si>
+  <si>
+    <t>Dar es Salaam</t>
+  </si>
+  <si>
+    <t>Mtwara</t>
+  </si>
+  <si>
+    <t>Maputo</t>
+  </si>
+  <si>
+    <t>Lilongwe</t>
+  </si>
+  <si>
+    <t>Polokwane</t>
+  </si>
+  <si>
+    <t>Limpopo</t>
+  </si>
+  <si>
+    <t>Durban</t>
+  </si>
+  <si>
+    <t>KwaZula-Natal</t>
+  </si>
+  <si>
+    <t>Port Elizabeth</t>
+  </si>
+  <si>
+    <t>Cape Of Good Hope</t>
+  </si>
+  <si>
+    <t>Cape Town</t>
+  </si>
+  <si>
+    <t>Johannesburg</t>
+  </si>
+  <si>
+    <t>Gauteng</t>
+  </si>
+  <si>
+    <t>Lubumbashi</t>
+  </si>
+  <si>
+    <t>Katanga</t>
+  </si>
+  <si>
+    <t>Equateur</t>
+  </si>
+  <si>
+    <t>Bandudu</t>
+  </si>
+  <si>
+    <t>Mbandaka</t>
+  </si>
+  <si>
+    <t>Bangui</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Lai</t>
+  </si>
+  <si>
+    <t>Tandjile</t>
+  </si>
+  <si>
+    <t>N'Djamena</t>
+  </si>
+  <si>
+    <t>Fada</t>
   </si>
 </sst>
 </file>
@@ -3469,11 +3634,11 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3535,15 +3700,15 @@
     <tableColumn id="6" xr3:uid="{70567373-7149-4072-B40C-F12E25F01158}" name="Capital" dataDxfId="11"/>
     <tableColumn id="9" xr3:uid="{50D709BB-24E3-418E-917C-1FC90D5E3D67}" name="Climate" dataDxfId="10"/>
     <tableColumn id="8" xr3:uid="{392E9EF2-6D86-4F40-BA63-FDDE5FAFA031}" name="Region" dataDxfId="9"/>
-    <tableColumn id="20" xr3:uid="{47D7ED67-4135-4227-A884-EB47174ED581}" name="Coastal Region" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{41CC5C72-302E-42DC-96EF-966AE29CDBEF}" name="Description" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{F90EBD04-4BA7-4952-A20B-2F9CB4512BCE}" name="City Population (Total)" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{8BF939FD-0C7E-4D5B-8550-48C36771ECB9}" name="National HDI" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{55A1BD7C-91C1-4086-B424-3AD1F292C066}" name="Culture Additive" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{49423110-5733-4638-B829-6BCE84E13431}" name="Culture Cost" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{16E85861-02C1-42B1-B650-7AE680AFBCB8}" name="Economic Cost" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{027A8570-4D49-4446-AD33-59BFA4DA3162}" name="Military Cost" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{160CCB0B-9916-4031-9F0D-50CB0E1AB6C7}" name="Score" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{47D7ED67-4135-4227-A884-EB47174ED581}" name="Coastal Region" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{41CC5C72-302E-42DC-96EF-966AE29CDBEF}" name="Description" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{F90EBD04-4BA7-4952-A20B-2F9CB4512BCE}" name="City Population (Total)" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{8BF939FD-0C7E-4D5B-8550-48C36771ECB9}" name="National HDI" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{55A1BD7C-91C1-4086-B424-3AD1F292C066}" name="Culture Additive" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{49423110-5733-4638-B829-6BCE84E13431}" name="Culture Cost" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{16E85861-02C1-42B1-B650-7AE680AFBCB8}" name="Economic Cost" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{027A8570-4D49-4446-AD33-59BFA4DA3162}" name="Military Cost" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{160CCB0B-9916-4031-9F0D-50CB0E1AB6C7}" name="Score" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3849,8 +4014,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H236" sqref="H236"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3950,7 +4115,9 @@
       <c r="H2" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>1096</v>
+      </c>
       <c r="J2" s="5"/>
       <c r="K2" s="3">
         <v>6000</v>
@@ -3987,7 +4154,9 @@
       <c r="H3" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>1096</v>
+      </c>
       <c r="J3" s="5"/>
       <c r="K3" s="3">
         <v>3200</v>
@@ -4024,7 +4193,9 @@
       <c r="H4" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>1096</v>
+      </c>
       <c r="J4" s="5"/>
       <c r="K4" s="3">
         <v>32000</v>
@@ -4061,7 +4232,9 @@
       <c r="H5" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>1096</v>
+      </c>
       <c r="J5" s="5"/>
       <c r="K5" s="3">
         <v>290000</v>
@@ -4098,7 +4271,9 @@
       <c r="H6" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>1096</v>
+      </c>
       <c r="J6" s="5"/>
       <c r="K6" s="3">
         <v>4200</v>
@@ -4135,7 +4310,9 @@
       <c r="H7" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>1096</v>
+      </c>
       <c r="J7" s="5"/>
       <c r="K7" s="3">
         <v>31000</v>
@@ -12694,14 +12871,20 @@
       <c r="E237" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F237" s="3"/>
+      <c r="F237" s="3" t="s">
+        <v>1097</v>
+      </c>
       <c r="G237" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="H237" s="3"/>
+      <c r="H237" s="3" t="s">
+        <v>1098</v>
+      </c>
       <c r="I237" s="3"/>
       <c r="J237" s="5"/>
-      <c r="K237" s="3"/>
+      <c r="K237" s="3">
+        <v>200000</v>
+      </c>
       <c r="L237" s="3"/>
       <c r="M237" s="3"/>
       <c r="N237" s="3"/>
@@ -12725,14 +12908,20 @@
       <c r="E238" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F238" s="3"/>
+      <c r="F238" s="3" t="s">
+        <v>1102</v>
+      </c>
       <c r="G238" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="H238" s="3"/>
+      <c r="H238" s="3" t="s">
+        <v>1100</v>
+      </c>
       <c r="I238" s="3"/>
       <c r="J238" s="5"/>
-      <c r="K238" s="3"/>
+      <c r="K238" s="3">
+        <v>480000</v>
+      </c>
       <c r="L238" s="3"/>
       <c r="M238" s="3"/>
       <c r="N238" s="3"/>
@@ -12756,14 +12945,20 @@
       <c r="E239" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F239" s="3"/>
+      <c r="F239" s="3" t="s">
+        <v>1099</v>
+      </c>
       <c r="G239" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="H239" s="3"/>
+      <c r="H239" s="3" t="s">
+        <v>1100</v>
+      </c>
       <c r="I239" s="3"/>
       <c r="J239" s="5"/>
-      <c r="K239" s="3"/>
+      <c r="K239" s="3">
+        <v>630000</v>
+      </c>
       <c r="L239" s="3"/>
       <c r="M239" s="3"/>
       <c r="N239" s="3"/>
@@ -12787,14 +12982,20 @@
       <c r="E240" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F240" s="3"/>
+      <c r="F240" s="3" t="s">
+        <v>1103</v>
+      </c>
       <c r="G240" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="H240" s="3"/>
+      <c r="H240" s="3" t="s">
+        <v>1100</v>
+      </c>
       <c r="I240" s="3"/>
       <c r="J240" s="5"/>
-      <c r="K240" s="3"/>
+      <c r="K240" s="3">
+        <v>410000</v>
+      </c>
       <c r="L240" s="3"/>
       <c r="M240" s="3"/>
       <c r="N240" s="3"/>
@@ -12855,14 +13056,20 @@
       <c r="E242" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F242" s="3"/>
+      <c r="F242" s="3" t="s">
+        <v>1104</v>
+      </c>
       <c r="G242" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="H242" s="3"/>
+      <c r="H242" s="3" t="s">
+        <v>1101</v>
+      </c>
       <c r="I242" s="3"/>
       <c r="J242" s="5"/>
-      <c r="K242" s="3"/>
+      <c r="K242" s="3">
+        <v>960000</v>
+      </c>
       <c r="L242" s="3"/>
       <c r="M242" s="3"/>
       <c r="N242" s="3"/>
@@ -12923,14 +13130,20 @@
       <c r="E244" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F244" s="3"/>
+      <c r="F244" s="3" t="s">
+        <v>1116</v>
+      </c>
       <c r="G244" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H244" s="3"/>
+      <c r="H244" s="3" t="s">
+        <v>1117</v>
+      </c>
       <c r="I244" s="3"/>
       <c r="J244" s="5"/>
-      <c r="K244" s="3"/>
+      <c r="K244" s="3">
+        <v>3300000</v>
+      </c>
       <c r="L244" s="3"/>
       <c r="M244" s="3"/>
       <c r="N244" s="3"/>
@@ -12954,14 +13167,20 @@
       <c r="E245" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F245" s="3"/>
+      <c r="F245" s="3" t="s">
+        <v>1119</v>
+      </c>
       <c r="G245" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H245" s="3"/>
+      <c r="H245" s="3" t="s">
+        <v>1118</v>
+      </c>
       <c r="I245" s="3"/>
       <c r="J245" s="5"/>
-      <c r="K245" s="3"/>
+      <c r="K245" s="3">
+        <v>760000</v>
+      </c>
       <c r="L245" s="3"/>
       <c r="M245" s="3"/>
       <c r="N245" s="3"/>
@@ -13022,14 +13241,20 @@
       <c r="E247" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F247" s="3"/>
+      <c r="F247" s="3" t="s">
+        <v>1120</v>
+      </c>
       <c r="G247" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H247" s="3"/>
+      <c r="H247" s="3" t="s">
+        <v>1121</v>
+      </c>
       <c r="I247" s="3"/>
       <c r="J247" s="5"/>
-      <c r="K247" s="3"/>
+      <c r="K247" s="3">
+        <v>920000</v>
+      </c>
       <c r="L247" s="3"/>
       <c r="M247" s="3"/>
       <c r="N247" s="3"/>
@@ -13053,14 +13278,20 @@
       <c r="E248" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F248" s="3"/>
+      <c r="F248" s="3" t="s">
+        <v>1126</v>
+      </c>
       <c r="G248" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H248" s="3"/>
+      <c r="H248" s="3" t="s">
+        <v>1123</v>
+      </c>
       <c r="I248" s="3"/>
       <c r="J248" s="5"/>
-      <c r="K248" s="3"/>
+      <c r="K248" s="3">
+        <v>1200000</v>
+      </c>
       <c r="L248" s="3"/>
       <c r="M248" s="3"/>
       <c r="N248" s="3"/>
@@ -13084,14 +13315,20 @@
       <c r="E249" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F249" s="3"/>
+      <c r="F249" s="3" t="s">
+        <v>1122</v>
+      </c>
       <c r="G249" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H249" s="3"/>
+      <c r="H249" s="3" t="s">
+        <v>1123</v>
+      </c>
       <c r="I249" s="3"/>
       <c r="J249" s="5"/>
-      <c r="K249" s="3"/>
+      <c r="K249" s="3">
+        <v>4300000</v>
+      </c>
       <c r="L249" s="3"/>
       <c r="M249" s="3"/>
       <c r="N249" s="3"/>
@@ -13115,14 +13352,20 @@
       <c r="E250" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F250" s="3"/>
+      <c r="F250" s="3" t="s">
+        <v>1128</v>
+      </c>
       <c r="G250" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H250" s="3"/>
+      <c r="H250" s="3" t="s">
+        <v>1124</v>
+      </c>
       <c r="I250" s="3"/>
       <c r="J250" s="5"/>
-      <c r="K250" s="3"/>
+      <c r="K250" s="3">
+        <v>100000</v>
+      </c>
       <c r="L250" s="3"/>
       <c r="M250" s="3"/>
       <c r="N250" s="3"/>
@@ -13146,14 +13389,20 @@
       <c r="E251" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F251" s="3"/>
+      <c r="F251" s="3" t="s">
+        <v>1127</v>
+      </c>
       <c r="G251" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H251" s="3"/>
+      <c r="H251" s="3" t="s">
+        <v>1124</v>
+      </c>
       <c r="I251" s="3"/>
       <c r="J251" s="5"/>
-      <c r="K251" s="3"/>
+      <c r="K251" s="3">
+        <v>7400000</v>
+      </c>
       <c r="L251" s="3"/>
       <c r="M251" s="3"/>
       <c r="N251" s="3"/>
@@ -13214,14 +13463,20 @@
       <c r="E253" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F253" s="3"/>
+      <c r="F253" s="3" t="s">
+        <v>1130</v>
+      </c>
       <c r="G253" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H253" s="3"/>
+      <c r="H253" s="3" t="s">
+        <v>1125</v>
+      </c>
       <c r="I253" s="3"/>
       <c r="J253" s="5"/>
-      <c r="K253" s="3"/>
+      <c r="K253" s="3">
+        <v>980000</v>
+      </c>
       <c r="L253" s="3"/>
       <c r="M253" s="3"/>
       <c r="N253" s="3"/>
@@ -13245,14 +13500,20 @@
       <c r="E254" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F254" s="3"/>
+      <c r="F254" s="3" t="s">
+        <v>1129</v>
+      </c>
       <c r="G254" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H254" s="3"/>
+      <c r="H254" s="3" t="s">
+        <v>1125</v>
+      </c>
       <c r="I254" s="3"/>
       <c r="J254" s="5"/>
-      <c r="K254" s="3"/>
+      <c r="K254" s="3">
+        <v>1000000</v>
+      </c>
       <c r="L254" s="3"/>
       <c r="M254" s="3"/>
       <c r="N254" s="3"/>
@@ -13350,14 +13611,20 @@
       <c r="E257" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F257" s="3"/>
+      <c r="F257" s="3" t="s">
+        <v>1131</v>
+      </c>
       <c r="G257" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H257" s="3"/>
+      <c r="H257" s="3" t="s">
+        <v>1132</v>
+      </c>
       <c r="I257" s="3"/>
       <c r="J257" s="5"/>
-      <c r="K257" s="3"/>
+      <c r="K257" s="3">
+        <v>130000</v>
+      </c>
       <c r="L257" s="3"/>
       <c r="M257" s="3"/>
       <c r="N257" s="3"/>
@@ -13381,14 +13648,20 @@
       <c r="E258" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F258" s="3"/>
+      <c r="F258" s="3" t="s">
+        <v>1133</v>
+      </c>
       <c r="G258" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H258" s="3"/>
+      <c r="H258" s="3" t="s">
+        <v>1134</v>
+      </c>
       <c r="I258" s="3"/>
       <c r="J258" s="5"/>
-      <c r="K258" s="3"/>
+      <c r="K258" s="3">
+        <v>3700000</v>
+      </c>
       <c r="L258" s="3"/>
       <c r="M258" s="3"/>
       <c r="N258" s="3"/>
@@ -13412,14 +13685,20 @@
       <c r="E259" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F259" s="3"/>
+      <c r="F259" s="3" t="s">
+        <v>1135</v>
+      </c>
       <c r="G259" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H259" s="3"/>
+      <c r="H259" s="3" t="s">
+        <v>1136</v>
+      </c>
       <c r="I259" s="3"/>
       <c r="J259" s="5"/>
-      <c r="K259" s="3"/>
+      <c r="K259" s="3">
+        <v>960000</v>
+      </c>
       <c r="L259" s="3"/>
       <c r="M259" s="3"/>
       <c r="N259" s="3"/>
@@ -13443,14 +13722,20 @@
       <c r="E260" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F260" s="3"/>
+      <c r="F260" s="3" t="s">
+        <v>1137</v>
+      </c>
       <c r="G260" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H260" s="3"/>
+      <c r="H260" s="3" t="s">
+        <v>1136</v>
+      </c>
       <c r="I260" s="3"/>
       <c r="J260" s="5"/>
-      <c r="K260" s="3"/>
+      <c r="K260" s="3">
+        <v>3700000</v>
+      </c>
       <c r="L260" s="3"/>
       <c r="M260" s="3"/>
       <c r="N260" s="3"/>
@@ -13474,14 +13759,20 @@
       <c r="E261" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F261" s="3"/>
+      <c r="F261" s="3" t="s">
+        <v>1138</v>
+      </c>
       <c r="G261" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="H261" s="3"/>
+      <c r="H261" s="3" t="s">
+        <v>1139</v>
+      </c>
       <c r="I261" s="3"/>
       <c r="J261" s="5"/>
-      <c r="K261" s="3"/>
+      <c r="K261" s="3">
+        <v>5600000</v>
+      </c>
       <c r="L261" s="3"/>
       <c r="M261" s="3"/>
       <c r="N261" s="3"/>
@@ -13616,14 +13907,20 @@
       <c r="E265" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F265" s="3"/>
+      <c r="F265" s="3" t="s">
+        <v>1140</v>
+      </c>
       <c r="G265" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="H265" s="3"/>
+      <c r="H265" s="3" t="s">
+        <v>1141</v>
+      </c>
       <c r="I265" s="3"/>
       <c r="J265" s="5"/>
-      <c r="K265" s="3"/>
+      <c r="K265" s="3">
+        <v>1700000</v>
+      </c>
       <c r="L265" s="3"/>
       <c r="M265" s="3"/>
       <c r="N265" s="3"/>
@@ -13647,14 +13944,20 @@
       <c r="E266" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F266" s="3"/>
+      <c r="F266" s="3" t="s">
+        <v>1143</v>
+      </c>
       <c r="G266" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="H266" s="3"/>
+      <c r="H266" s="3" t="s">
+        <v>1143</v>
+      </c>
       <c r="I266" s="3"/>
       <c r="J266" s="5"/>
-      <c r="K266" s="3"/>
+      <c r="K266" s="3">
+        <v>140000</v>
+      </c>
       <c r="L266" s="3"/>
       <c r="M266" s="3"/>
       <c r="N266" s="3"/>
@@ -13715,14 +14018,20 @@
       <c r="E268" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F268" s="3"/>
+      <c r="F268" s="3" t="s">
+        <v>1144</v>
+      </c>
       <c r="G268" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="H268" s="3"/>
+      <c r="H268" s="3" t="s">
+        <v>1142</v>
+      </c>
       <c r="I268" s="3"/>
       <c r="J268" s="5"/>
-      <c r="K268" s="3"/>
+      <c r="K268" s="3">
+        <v>1100000</v>
+      </c>
       <c r="L268" s="3"/>
       <c r="M268" s="3"/>
       <c r="N268" s="3"/>
@@ -13746,14 +14055,20 @@
       <c r="E269" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F269" s="3"/>
+      <c r="F269" s="3" t="s">
+        <v>1145</v>
+      </c>
       <c r="G269" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="H269" s="3"/>
+      <c r="H269" s="3" t="s">
+        <v>1146</v>
+      </c>
       <c r="I269" s="3"/>
       <c r="J269" s="5"/>
-      <c r="K269" s="3"/>
+      <c r="K269" s="3">
+        <v>700000</v>
+      </c>
       <c r="L269" s="3"/>
       <c r="M269" s="3"/>
       <c r="N269" s="3"/>
@@ -13777,14 +14092,20 @@
       <c r="E270" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F270" s="3"/>
+      <c r="F270" s="3" t="s">
+        <v>1147</v>
+      </c>
       <c r="G270" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H270" s="3"/>
+      <c r="H270" s="3" t="s">
+        <v>1148</v>
+      </c>
       <c r="I270" s="3"/>
       <c r="J270" s="5"/>
-      <c r="K270" s="3"/>
+      <c r="K270" s="3">
+        <v>20000</v>
+      </c>
       <c r="L270" s="3"/>
       <c r="M270" s="3"/>
       <c r="N270" s="3"/>
@@ -13808,14 +14129,20 @@
       <c r="E271" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F271" s="3"/>
+      <c r="F271" s="3" t="s">
+        <v>1150</v>
+      </c>
       <c r="G271" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H271" s="3"/>
+      <c r="H271" s="3" t="s">
+        <v>1150</v>
+      </c>
       <c r="I271" s="3"/>
       <c r="J271" s="5"/>
-      <c r="K271" s="3"/>
+      <c r="K271" s="3">
+        <v>23000</v>
+      </c>
       <c r="L271" s="3"/>
       <c r="M271" s="3"/>
       <c r="N271" s="3"/>
@@ -13839,14 +14166,20 @@
       <c r="E272" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F272" s="3"/>
+      <c r="F272" s="3" t="s">
+        <v>1149</v>
+      </c>
       <c r="G272" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H272" s="3"/>
+      <c r="H272" s="3" t="s">
+        <v>1149</v>
+      </c>
       <c r="I272" s="3"/>
       <c r="J272" s="5"/>
-      <c r="K272" s="3"/>
+      <c r="K272" s="3">
+        <v>950000</v>
+      </c>
       <c r="L272" s="3"/>
       <c r="M272" s="3"/>
       <c r="N272" s="3"/>
@@ -13907,14 +14240,20 @@
       <c r="E274" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F274" s="3"/>
+      <c r="F274" s="3" t="s">
+        <v>1105</v>
+      </c>
       <c r="G274" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="H274" s="3"/>
+      <c r="H274" s="3" t="s">
+        <v>1106</v>
+      </c>
       <c r="I274" s="3"/>
       <c r="J274" s="5"/>
-      <c r="K274" s="3"/>
+      <c r="K274" s="3">
+        <v>2700000</v>
+      </c>
       <c r="L274" s="3"/>
       <c r="M274" s="3"/>
       <c r="N274" s="3"/>
@@ -15461,14 +15800,20 @@
       <c r="E322" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F322" s="3"/>
+      <c r="F322" s="3" t="s">
+        <v>1113</v>
+      </c>
       <c r="G322" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="H322" s="3"/>
+      <c r="H322" s="3" t="s">
+        <v>1114</v>
+      </c>
       <c r="I322" s="3"/>
       <c r="J322" s="5"/>
-      <c r="K322" s="3"/>
+      <c r="K322" s="3">
+        <v>1100000</v>
+      </c>
       <c r="L322" s="3"/>
       <c r="M322" s="3"/>
       <c r="N322" s="3"/>
@@ -15492,14 +15837,20 @@
       <c r="E323" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F323" s="3"/>
+      <c r="F323" s="3" t="s">
+        <v>1115</v>
+      </c>
       <c r="G323" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="H323" s="3"/>
+      <c r="H323" s="3" t="s">
+        <v>1114</v>
+      </c>
       <c r="I323" s="3"/>
       <c r="J323" s="5"/>
-      <c r="K323" s="3"/>
+      <c r="K323" s="3">
+        <v>190000</v>
+      </c>
       <c r="L323" s="3"/>
       <c r="M323" s="3"/>
       <c r="N323" s="3"/>
@@ -18132,14 +18483,20 @@
       <c r="E397" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F397" s="3"/>
+      <c r="F397" s="3" t="s">
+        <v>1111</v>
+      </c>
       <c r="G397" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H397" s="3"/>
+      <c r="H397" s="3" t="s">
+        <v>1112</v>
+      </c>
       <c r="I397" s="3"/>
       <c r="J397" s="5"/>
-      <c r="K397" s="3"/>
+      <c r="K397" s="3">
+        <v>940000</v>
+      </c>
       <c r="L397" s="3"/>
       <c r="M397" s="3"/>
       <c r="N397" s="3"/>
@@ -18163,14 +18520,20 @@
       <c r="E398" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F398" s="3"/>
+      <c r="F398" s="3" t="s">
+        <v>1109</v>
+      </c>
       <c r="G398" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="H398" s="3"/>
+      <c r="H398" s="3" t="s">
+        <v>1110</v>
+      </c>
       <c r="I398" s="3"/>
       <c r="J398" s="5"/>
-      <c r="K398" s="3"/>
+      <c r="K398" s="3">
+        <v>2200000</v>
+      </c>
       <c r="L398" s="3"/>
       <c r="M398" s="3"/>
       <c r="N398" s="3"/>
@@ -18287,14 +18650,20 @@
       <c r="E402" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F402" s="3"/>
+      <c r="F402" s="3" t="s">
+        <v>1107</v>
+      </c>
       <c r="G402" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="H402" s="3"/>
+      <c r="H402" s="3" t="s">
+        <v>1108</v>
+      </c>
       <c r="I402" s="3"/>
       <c r="J402" s="5"/>
-      <c r="K402" s="3"/>
+      <c r="K402" s="3">
+        <v>1800000</v>
+      </c>
       <c r="L402" s="3"/>
       <c r="M402" s="3"/>
       <c r="N402" s="3"/>

</xml_diff>